<commit_message>
listo el punto 5
</commit_message>
<xml_diff>
--- a/hipotesis/HIPOTESIS vs VARIABLES.xlsx
+++ b/hipotesis/HIPOTESIS vs VARIABLES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/MCD/proyectodegrado2/hipotesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27408BDB-3DD7-7241-B63E-639187A9FCB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DE7CFA-055E-BF44-8FFC-E6A5EFB2326B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15360" yWindow="1600" windowWidth="51200" windowHeight="26620" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>Nulos</t>
   </si>
   <si>
-    <t>nivel_hace_YY</t>
-  </si>
-  <si>
     <t>YY: hace cuantos semestres</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
   </si>
   <si>
     <t>promedio nivel nota obtenido por departamentos en semestres anteriores</t>
-  </si>
-  <si>
-    <t>nivel_dpto_YY</t>
   </si>
   <si>
     <t>promedio nivel nota obtenido por asignatura en semestres anteriores</t>
@@ -399,6 +393,12 @@
   </si>
   <si>
     <t>-100 si no se encontró esa área del estudainte en icfes</t>
+  </si>
+  <si>
+    <t>prom_nivel_hace_YY</t>
+  </si>
+  <si>
+    <t>prom_nivel_dpto_YY</t>
   </si>
 </sst>
 </file>
@@ -856,7 +856,7 @@
   <dimension ref="A1:K67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -878,10 +878,10 @@
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>7</v>
@@ -911,13 +911,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>54</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>56</v>
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
@@ -928,16 +928,16 @@
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="G4" s="19" t="s">
         <v>108</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -945,17 +945,17 @@
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -966,10 +966,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>9</v>
@@ -978,41 +978,49 @@
         <v>11</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>2</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>15</v>
+      <c r="B7" s="15">
+        <v>3</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>3</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="9" t="s">
+      <c r="B8" s="15">
+        <v>4</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="17" t="s">
         <v>15</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -1020,16 +1028,16 @@
         <v>4</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="G9" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1037,16 +1045,16 @@
         <v>5</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1054,16 +1062,16 @@
         <v>6</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="G11" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -1071,10 +1079,10 @@
         <v>7</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="9">
@@ -1086,10 +1094,10 @@
         <v>8</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="9">
@@ -1101,10 +1109,10 @@
         <v>9</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="9">
@@ -1116,13 +1124,13 @@
         <v>10</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G15" s="9">
         <v>0</v>
@@ -1133,13 +1141,13 @@
         <v>11</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G16" s="9">
         <v>0</v>
@@ -1150,16 +1158,16 @@
         <v>12</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="G17" s="9" t="s">
         <v>97</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1167,17 +1175,17 @@
         <v>13</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1185,13 +1193,13 @@
         <v>14</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G19" s="5">
         <v>0</v>
@@ -1202,13 +1210,13 @@
         <v>15</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G20" s="5">
         <v>0</v>
@@ -1219,13 +1227,13 @@
         <v>16</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G21" s="5">
         <v>0</v>
@@ -1236,17 +1244,17 @@
         <v>17</v>
       </c>
       <c r="C22" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1254,13 +1262,13 @@
         <v>18</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>87</v>
       </c>
       <c r="G23" s="5">
         <v>0</v>
@@ -1271,13 +1279,13 @@
         <v>19</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="G24" s="5">
         <v>0</v>
@@ -1288,13 +1296,13 @@
         <v>20</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5">
@@ -1307,10 +1315,10 @@
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5">
@@ -1323,13 +1331,13 @@
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G27" s="5">
         <v>0</v>
@@ -1341,13 +1349,13 @@
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="G28" s="5">
         <v>0</v>
@@ -1359,13 +1367,13 @@
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G29" s="5">
         <v>0</v>
@@ -1389,17 +1397,17 @@
         <v>0</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F31" s="17"/>
       <c r="G31" s="19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1411,14 +1419,14 @@
       </c>
       <c r="C32" s="16"/>
       <c r="D32" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1430,16 +1438,16 @@
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E33" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G33" s="17" t="s">
         <v>101</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="G33" s="17" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1450,17 +1458,17 @@
         <v>0</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1472,14 +1480,14 @@
       </c>
       <c r="C35" s="16"/>
       <c r="D35" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1487,13 +1495,13 @@
         <v>31</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5">
@@ -1506,10 +1514,10 @@
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5">
@@ -1521,13 +1529,13 @@
         <v>33</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5">
@@ -1539,16 +1547,16 @@
         <v>34</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1559,7 +1567,7 @@
     </row>
     <row r="41" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="C41" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>

</xml_diff>

<commit_message>
ya vamos en 11
</commit_message>
<xml_diff>
--- a/hipotesis/HIPOTESIS vs VARIABLES.xlsx
+++ b/hipotesis/HIPOTESIS vs VARIABLES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/MCD/proyectodegrado2/hipotesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB04552B-7137-B249-83C9-C6A29B7397B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C06D0E8-1E48-2840-8B51-FA21CC1C0860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="1600" windowWidth="51200" windowHeight="26620" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
+    <workbookView xWindow="18260" yWindow="1100" windowWidth="32180" windowHeight="25300" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="124">
   <si>
     <t>Variables</t>
   </si>
@@ -161,9 +161,6 @@
     <t>cantidad de cursos que había tomado en CURSOS DE VERANO antes de tomar este curso?</t>
   </si>
   <si>
-    <t>cuales cursos había tomado en curso de verano?</t>
-  </si>
-  <si>
     <t>ultima nota obtenida en asignaturas vistas antes</t>
   </si>
   <si>
@@ -171,12 +168,6 @@
   </si>
   <si>
     <t>q_cursos_tomados</t>
-  </si>
-  <si>
-    <t>q_cursos_en_CV</t>
-  </si>
-  <si>
-    <t>asig_en_CV_YY</t>
   </si>
   <si>
     <t>YY: asignatura</t>
@@ -399,6 +390,29 @@
   </si>
   <si>
     <t>q_semestres_reg_tomados</t>
+  </si>
+  <si>
+    <t>cuales cursos había tomado en curso de verano y con que profe?</t>
+  </si>
+  <si>
+    <t>cantidad de cursos de vernao por dpto</t>
+  </si>
+  <si>
+    <t>q_cursos_CV</t>
+  </si>
+  <si>
+    <t>q_cursos_CV_dpto_YY</t>
+  </si>
+  <si>
+    <t>asig_en_CV_YY_XX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YY: asignatura
+</t>
+  </si>
+  <si>
+    <t>YY:asignatura
+XX: profe</t>
   </si>
 </sst>
 </file>
@@ -853,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39A78E9-D45D-3D4E-A52F-2B0492CA372F}">
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:G13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -878,10 +892,10 @@
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>7</v>
@@ -911,13 +925,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
@@ -928,16 +942,16 @@
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" s="19" t="s">
         <v>102</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -945,17 +959,17 @@
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -969,7 +983,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>9</v>
@@ -978,7 +992,7 @@
         <v>11</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="51" x14ac:dyDescent="0.2">
@@ -993,10 +1007,10 @@
         <v>21</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G7" s="19" t="s">
         <v>14</v>
@@ -1014,10 +1028,10 @@
         <v>15</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G8" s="19" t="s">
         <v>14</v>
@@ -1035,7 +1049,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>17</v>
@@ -1049,10 +1063,10 @@
         <v>5</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>17</v>
@@ -1073,7 +1087,7 @@
         <v>19</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>20</v>
@@ -1094,7 +1108,7 @@
         <v>36</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="19">
@@ -1113,7 +1127,7 @@
         <v>37</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="19">
@@ -1124,115 +1138,121 @@
       <c r="A14" s="4">
         <v>9</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="B14" s="15">
+        <v>9</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="9">
+      <c r="E14" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
+      <c r="B15" s="15">
         <v>10</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="C15" s="15"/>
+      <c r="D15" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
+        <v>10</v>
+      </c>
+      <c r="B16" s="4">
         <v>11</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>75</v>
+        <v>121</v>
       </c>
       <c r="F16" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>11</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G17" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>12</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>13</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G16" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
-        <v>12</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
-        <v>13</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
-        <v>14</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" s="5">
-        <v>0</v>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G20" s="5">
         <v>0</v>
@@ -1240,300 +1260,301 @@
     </row>
     <row r="21" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
+        <v>15</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
         <v>16</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
-        <v>17</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="E22" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5" t="s">
-        <v>90</v>
+        <v>54</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G23" s="5">
-        <v>0</v>
+        <v>76</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
+        <v>18</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
         <v>19</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G24" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
+      <c r="D25" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
         <v>20</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
-        <v>21</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="E26" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="5" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>52</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F27" s="5"/>
       <c r="G27" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="G28" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>24</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G29" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
+      <c r="G30" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
         <v>25</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="4">
-        <v>26</v>
-      </c>
-      <c r="B31" s="15">
-        <v>0</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31" s="17"/>
-      <c r="G31" s="19" t="s">
-        <v>111</v>
-      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="15">
         <v>0</v>
       </c>
-      <c r="C32" s="16"/>
+      <c r="C32" s="16" t="s">
+        <v>23</v>
+      </c>
       <c r="D32" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="19" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33" s="15">
         <v>0</v>
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="17" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="G33" s="17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="F33" s="17"/>
+      <c r="G33" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
+        <v>28</v>
+      </c>
+      <c r="B34" s="15">
+        <v>0</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
         <v>29</v>
       </c>
-      <c r="B34" s="15">
-        <v>0</v>
-      </c>
-      <c r="C34" s="16" t="s">
+      <c r="B35" s="15">
+        <v>0</v>
+      </c>
+      <c r="C35" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D35" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E34" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="F34" s="17"/>
-      <c r="G34" s="19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="4">
-        <v>30</v>
-      </c>
-      <c r="B35" s="15">
-        <v>0</v>
-      </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="17" t="s">
-        <v>27</v>
-      </c>
       <c r="E35" s="17" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="19" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
-        <v>31</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="B36" s="15">
+        <v>0</v>
+      </c>
+      <c r="C36" s="16"/>
+      <c r="D36" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="F36" s="17"/>
+      <c r="G36" s="19" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
-        <v>32</v>
-      </c>
-      <c r="C37" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="D37" s="5" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5">
@@ -1542,16 +1563,14 @@
     </row>
     <row r="38" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
-        <v>33</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>38</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C38" s="7"/>
       <c r="D38" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5">
@@ -1560,46 +1579,55 @@
     </row>
     <row r="39" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
+        <v>33</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
         <v>34</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F39" s="5" t="s">
+      <c r="D40" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G39" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-    </row>
-    <row r="41" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="C41" s="5" t="s">
-        <v>60</v>
-      </c>
+      <c r="G40" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="C42" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C43" s="10" t="s">
-        <v>1</v>
-      </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
@@ -1607,7 +1635,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C44" s="10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
@@ -1615,7 +1643,9 @@
       <c r="G44" s="5"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C45" s="10"/>
+      <c r="C45" s="10" t="s">
+        <v>2</v>
+      </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -1629,9 +1659,7 @@
       <c r="G46" s="5"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C47" s="10" t="s">
-        <v>3</v>
-      </c>
+      <c r="C47" s="10"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -1639,7 +1667,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C48" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
@@ -1648,7 +1676,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C49" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
@@ -1657,20 +1685,21 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C50" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="11"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-      <c r="E59"/>
-      <c r="F59"/>
-      <c r="G59"/>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C51" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="11"/>
@@ -1732,12 +1761,21 @@
       <c r="A67" s="11"/>
       <c r="B67" s="11"/>
       <c r="C67" s="11"/>
-      <c r="D67" s="10"/>
       <c r="E67"/>
       <c r="F67"/>
       <c r="G67"/>
     </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="11"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="10"/>
+      <c r="E68"/>
+      <c r="F68"/>
+      <c r="G68"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se revisó todo transformacion de datos y se encontraron errores pues no se había contemplado correctamente el concepto de los esutdiante que apenas estaban viendo las asiganturas en fuestion, pues venian con nota cero..   el analisis indicó que realmente había que asumir que tenian nota nula.  eso cambio muchas cosas y hbuo que revisarlos todo
</commit_message>
<xml_diff>
--- a/hipotesis/HIPOTESIS vs VARIABLES.xlsx
+++ b/hipotesis/HIPOTESIS vs VARIABLES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/MCD/proyectodegrado2/hipotesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C06D0E8-1E48-2840-8B51-FA21CC1C0860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4883F1B4-2E5C-8A42-8BD8-2DC78527EA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18260" yWindow="1100" windowWidth="32180" windowHeight="25300" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
+    <workbookView xWindow="18260" yWindow="1060" windowWidth="32180" windowHeight="25300" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -392,9 +392,6 @@
     <t>q_semestres_reg_tomados</t>
   </si>
   <si>
-    <t>cuales cursos había tomado en curso de verano y con que profe?</t>
-  </si>
-  <si>
     <t>cantidad de cursos de vernao por dpto</t>
   </si>
   <si>
@@ -402,17 +399,19 @@
   </si>
   <si>
     <t>q_cursos_CV_dpto_YY</t>
-  </si>
-  <si>
-    <t>asig_en_CV_YY_XX</t>
   </si>
   <si>
     <t xml:space="preserve">YY: asignatura
 </t>
   </si>
   <si>
-    <t>YY:asignatura
-XX: profe</t>
+    <t>cantidad de cursos tomado en CV por docente</t>
+  </si>
+  <si>
+    <t>XX: id_docente</t>
+  </si>
+  <si>
+    <t>q_cursos_CV_docente_XX</t>
   </si>
 </sst>
 </file>
@@ -870,7 +869,7 @@
   <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1146,7 +1145,7 @@
         <v>40</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="19">
@@ -1159,33 +1158,36 @@
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F15" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="G15" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>10</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="15">
         <v>11</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="E16" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="G16" s="9">
+      <c r="F16" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" s="19">
         <v>0</v>
       </c>
     </row>
@@ -1200,7 +1202,7 @@
         <v>72</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G17" s="9">
         <v>0</v>

</xml_diff>

<commit_message>
ya vamos por el punto 12
</commit_message>
<xml_diff>
--- a/hipotesis/HIPOTESIS vs VARIABLES.xlsx
+++ b/hipotesis/HIPOTESIS vs VARIABLES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/MCD/proyectodegrado2/hipotesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4883F1B4-2E5C-8A42-8BD8-2DC78527EA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FD1419-A293-2F4A-AE49-34175E005A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18260" yWindow="1060" windowWidth="32180" windowHeight="25300" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
   </bookViews>
@@ -868,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39A78E9-D45D-3D4E-A52F-2B0492CA372F}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1195,20 +1195,24 @@
       <c r="A17" s="4">
         <v>11</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="B17" s="15">
+        <v>12</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="G17" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="G17" s="19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>12</v>
       </c>
@@ -1221,8 +1225,8 @@
       <c r="F18" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>91</v>
+      <c r="G18" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
listo el punto 15
</commit_message>
<xml_diff>
--- a/hipotesis/HIPOTESIS vs VARIABLES.xlsx
+++ b/hipotesis/HIPOTESIS vs VARIABLES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/MCD/proyectodegrado2/hipotesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DB4120-07D6-9941-AF16-4F34F8F4D3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA7EA33-A23E-0B4B-A6FC-C17A7963E99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18260" yWindow="1060" windowWidth="32180" windowHeight="25300" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
   </bookViews>
@@ -869,7 +869,7 @@
   <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B21" sqref="B21:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1254,16 +1254,20 @@
       <c r="A20" s="4">
         <v>14</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="B20" s="15">
+        <v>14</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="17">
         <v>0</v>
       </c>
     </row>
@@ -1271,16 +1275,20 @@
       <c r="A21" s="4">
         <v>15</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="B21" s="15">
+        <v>15</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="17">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
vamos por punto 22
</commit_message>
<xml_diff>
--- a/hipotesis/HIPOTESIS vs VARIABLES.xlsx
+++ b/hipotesis/HIPOTESIS vs VARIABLES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/MCD/proyectodegrado2/hipotesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC79E699-08C7-494B-B338-08A25C1FE9B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7777D19E-D6B3-5A4B-B8FF-ED699D6087F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18260" yWindow="1040" windowWidth="32180" windowHeight="25300" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
+    <workbookView xWindow="19820" yWindow="1220" windowWidth="32180" windowHeight="25300" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="120">
   <si>
     <t>Variables</t>
   </si>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>cuantas veces ya había visto la asignatura que está matriculando</t>
-  </si>
-  <si>
-    <t>cuantas veces ya había repetido otras asignaturas</t>
   </si>
   <si>
     <t>tamaño del curso actual</t>
@@ -214,31 +211,10 @@
     <t>* Heterogeniedad cursos anteriores no es posible porque solo me dieron data de los cursos que tomó un estudiante que tomó 300MAG006 o 007.  ASI QUE NO SE SABE cómo estaban compuestos esos grupos</t>
   </si>
   <si>
-    <t>curso_actual_repeticiones</t>
-  </si>
-  <si>
-    <t>otros_cursos_repeticiones</t>
-  </si>
-  <si>
-    <t>otros_cursos_repe_hace_YY</t>
-  </si>
-  <si>
-    <t>cantidad cursos repetidos en semestres anteriores</t>
-  </si>
-  <si>
     <t>cantidad cursos repetidos por departamento en semestres antreiores</t>
   </si>
   <si>
-    <t>otros_cursos_repe_dpto_YY</t>
-  </si>
-  <si>
     <t>YY:dpto</t>
-  </si>
-  <si>
-    <t>cantidad de veces que repitió ciertas asignaturas</t>
-  </si>
-  <si>
-    <t>otros_cursos_repe_asig_YY</t>
   </si>
   <si>
     <t>estudiante_edad</t>
@@ -412,6 +388,18 @@
   </si>
   <si>
     <t>q_cursos_CV_docente_XX</t>
+  </si>
+  <si>
+    <t>cuantas asignaturas ya había perdido o cancelado antes de tomar esta asignatura?</t>
+  </si>
+  <si>
+    <t>cursos_per_canc_antes</t>
+  </si>
+  <si>
+    <t>cursos_per_canc_antes_otros</t>
+  </si>
+  <si>
+    <t>cursos_per_canc_antes_otros_dpto_YY</t>
   </si>
 </sst>
 </file>
@@ -866,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39A78E9-D45D-3D4E-A52F-2B0492CA372F}">
-  <dimension ref="A1:K68"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:G25"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -891,10 +879,10 @@
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>7</v>
@@ -924,13 +912,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>47</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>48</v>
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
@@ -941,16 +929,16 @@
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -958,17 +946,17 @@
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="14" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -982,7 +970,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>9</v>
@@ -991,7 +979,7 @@
         <v>11</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="51" x14ac:dyDescent="0.2">
@@ -1006,10 +994,10 @@
         <v>21</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G7" s="19" t="s">
         <v>14</v>
@@ -1027,10 +1015,10 @@
         <v>15</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G8" s="19" t="s">
         <v>14</v>
@@ -1048,7 +1036,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>17</v>
@@ -1062,10 +1050,10 @@
         <v>5</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>17</v>
@@ -1086,7 +1074,7 @@
         <v>19</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>20</v>
@@ -1104,10 +1092,10 @@
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="19">
@@ -1123,10 +1111,10 @@
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="19">
@@ -1142,10 +1130,10 @@
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="19">
@@ -1158,13 +1146,13 @@
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="17" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G15" s="19">
         <v>0</v>
@@ -1179,13 +1167,13 @@
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="17" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="G16" s="19">
         <v>0</v>
@@ -1200,16 +1188,16 @@
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="17" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1217,13 +1205,13 @@
         <v>12</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G18" s="3">
         <v>0</v>
@@ -1237,17 +1225,17 @@
         <v>13</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1259,13 +1247,13 @@
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G20" s="17">
         <v>0</v>
@@ -1280,13 +1268,13 @@
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G21" s="17">
         <v>0</v>
@@ -1301,13 +1289,13 @@
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G22" s="17">
         <v>0</v>
@@ -1321,17 +1309,17 @@
         <v>17</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="17" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1343,13 +1331,13 @@
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="17" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G24" s="17">
         <v>0</v>
@@ -1364,13 +1352,13 @@
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="17" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G25" s="17">
         <v>0</v>
@@ -1380,213 +1368,220 @@
       <c r="A26" s="4">
         <v>20</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="B26" s="15">
+        <v>20</v>
+      </c>
+      <c r="C26" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="E26" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>21</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="B27" s="15">
+        <v>21</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
+        <v>23</v>
+      </c>
+      <c r="B28" s="15">
         <v>22</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G28" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="C28" s="16"/>
+      <c r="D28" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C29" s="7"/>
-      <c r="D29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G29" s="5">
-        <v>0</v>
-      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
-        <v>24</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="B30" s="15">
+        <v>0</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="17"/>
+      <c r="G30" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
-        <v>25</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="B31" s="15">
+        <v>0</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="19" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B32" s="15">
         <v>0</v>
       </c>
-      <c r="C32" s="16" t="s">
-        <v>23</v>
-      </c>
+      <c r="C32" s="16"/>
       <c r="D32" s="17" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B33" s="15">
         <v>0</v>
       </c>
-      <c r="C33" s="16"/>
+      <c r="C33" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="D33" s="17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="F33" s="17"/>
       <c r="G33" s="19" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B34" s="15">
         <v>0</v>
       </c>
       <c r="C34" s="16"/>
       <c r="D34" s="17" t="s">
-        <v>83</v>
+        <v>27</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>95</v>
+        <v>88</v>
+      </c>
+      <c r="F34" s="17"/>
+      <c r="G34" s="19" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
-        <v>29</v>
-      </c>
-      <c r="B35" s="15">
-        <v>0</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="F35" s="17"/>
-      <c r="G35" s="19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
-        <v>30</v>
-      </c>
-      <c r="B36" s="15">
-        <v>0</v>
-      </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="F36" s="17"/>
-      <c r="G36" s="19" t="s">
-        <v>110</v>
+        <v>32</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5">
@@ -1595,54 +1590,35 @@
     </row>
     <row r="38" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
-        <v>32</v>
-      </c>
-      <c r="C38" s="7"/>
+        <v>34</v>
+      </c>
       <c r="D38" s="5" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A39" s="4">
-        <v>33</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>71</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="4">
-        <v>34</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>98</v>
-      </c>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="C40" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D41" s="5"/>
@@ -1650,9 +1626,9 @@
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="C42" s="5" t="s">
-        <v>57</v>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C42" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
@@ -1660,38 +1636,41 @@
       <c r="G42" s="5"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C43" s="10" t="s">
+        <v>2</v>
+      </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C44" s="10" t="s">
-        <v>1</v>
-      </c>
+      <c r="C44" s="10"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C45" s="10" t="s">
-        <v>2</v>
-      </c>
+      <c r="C45" s="10"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C46" s="10"/>
+      <c r="C46" s="10" t="s">
+        <v>3</v>
+      </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C47" s="10"/>
+      <c r="C47" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -1699,7 +1678,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C48" s="10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
@@ -1708,30 +1687,28 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C49" s="10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C50" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C51" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="11"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="E58"/>
+      <c r="F58"/>
+      <c r="G58"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="11"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="E59"/>
+      <c r="F59"/>
+      <c r="G59"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="11"/>
@@ -1785,26 +1762,10 @@
       <c r="A66" s="11"/>
       <c r="B66" s="11"/>
       <c r="C66" s="11"/>
+      <c r="D66" s="10"/>
       <c r="E66"/>
       <c r="F66"/>
       <c r="G66"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="11"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="11"/>
-      <c r="E67"/>
-      <c r="F67"/>
-      <c r="G67"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="11"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="10"/>
-      <c r="E68"/>
-      <c r="F68"/>
-      <c r="G68"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
terminé todas las transformaciones e inicié a crear DATOS_LIMPIOS
</commit_message>
<xml_diff>
--- a/hipotesis/HIPOTESIS vs VARIABLES.xlsx
+++ b/hipotesis/HIPOTESIS vs VARIABLES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/MCD/proyectodegrado2/hipotesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7777D19E-D6B3-5A4B-B8FF-ED699D6087F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB623382-A79F-8F43-A0A7-0C586CC45CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19820" yWindow="1220" windowWidth="32180" windowHeight="25300" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="115">
   <si>
     <t>Variables</t>
   </si>
@@ -140,9 +140,6 @@
     <t>composicion del curso actual por programa del que vienen los estudiantes</t>
   </si>
   <si>
-    <t>al momento de dictar el curso, cuantos cursos había dictado en otras asignaturas</t>
-  </si>
-  <si>
     <t>cuantos cursos ya había tomado el estudiante antes de tomar el curso actual?</t>
   </si>
   <si>
@@ -156,12 +153,6 @@
   </si>
   <si>
     <t>cantidad de cursos que había tomado en CURSOS DE VERANO antes de tomar este curso?</t>
-  </si>
-  <si>
-    <t>ultima nota obtenida en asignaturas vistas antes</t>
-  </si>
-  <si>
-    <t>nivel_asig_ultima_YY</t>
   </si>
   <si>
     <t>q_cursos_tomados</t>
@@ -280,15 +271,6 @@
     <t>ERROR si &lt; 1</t>
   </si>
   <si>
-    <t>docente con que tomó ultima vez cursos</t>
-  </si>
-  <si>
-    <t>curso_tomado_ult_docente_YY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YY: asig </t>
-  </si>
-  <si>
     <t>-10 significa que no tomó ese curso con ese docente</t>
   </si>
   <si>
@@ -400,6 +382,9 @@
   </si>
   <si>
     <t>cursos_per_canc_antes_otros_dpto_YY</t>
+  </si>
+  <si>
+    <t>al momento de dictar el curso, cuantos cursos había dictado en cualquier otra asignaturas</t>
   </si>
 </sst>
 </file>
@@ -478,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -498,14 +483,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -854,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39A78E9-D45D-3D4E-A52F-2B0492CA372F}">
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -872,17 +851,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>7</v>
@@ -906,714 +885,716 @@
     </row>
     <row r="3" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>0</v>
-      </c>
-      <c r="B3" s="15">
-        <v>0</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="B3" s="13">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="B4" s="15">
-        <v>0</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17" t="s">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="18">
+        <v>1</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12" t="s">
         <v>91</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="B5" s="20">
-        <v>1</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>1</v>
-      </c>
-      <c r="B6" s="15">
+        <v>4</v>
+      </c>
+      <c r="B6" s="13">
         <v>2</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="17" t="s">
+      <c r="D6" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="19" t="s">
-        <v>103</v>
+      <c r="G6" s="17" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <v>2</v>
-      </c>
-      <c r="B7" s="15">
+        <v>5</v>
+      </c>
+      <c r="B7" s="13">
         <v>3</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="17" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" s="19" t="s">
+      <c r="E7" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <v>3</v>
-      </c>
-      <c r="B8" s="15">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13">
         <v>4</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="17" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="19" t="s">
+      <c r="E8" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
-        <v>4</v>
-      </c>
-      <c r="B9" s="15">
+        <v>7</v>
+      </c>
+      <c r="B9" s="13">
         <v>5</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="17" t="s">
+      <c r="C9" s="13"/>
+      <c r="D9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="17" t="s">
+      <c r="E9" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>5</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="13">
+        <v>6</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <v>6</v>
-      </c>
-      <c r="B11" s="15">
-        <v>6</v>
-      </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="B11" s="13">
+        <v>7</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <v>7</v>
-      </c>
-      <c r="B12" s="15">
-        <v>7</v>
-      </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="13">
+        <v>8</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="19">
+      <c r="E12" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <v>8</v>
-      </c>
-      <c r="B13" s="15">
-        <v>8</v>
-      </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="13">
+        <v>9</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>12</v>
+      </c>
+      <c r="B14" s="13">
+        <v>10</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>13</v>
+      </c>
+      <c r="B15" s="13">
+        <v>11</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
-        <v>9</v>
-      </c>
-      <c r="B14" s="15">
-        <v>9</v>
-      </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="B15" s="15">
-        <v>10</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="G15" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <v>10</v>
-      </c>
-      <c r="B16" s="15">
-        <v>11</v>
-      </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="G16" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="13">
+        <v>12</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
-        <v>11</v>
-      </c>
-      <c r="B17" s="15">
-        <v>12</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="13">
+        <v>13</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
-        <v>12</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="13">
+        <v>14</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
-        <v>13</v>
-      </c>
-      <c r="B19" s="15">
-        <v>13</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17" t="s">
-        <v>79</v>
+        <v>17</v>
+      </c>
+      <c r="B19" s="13">
+        <v>15</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>14</v>
-      </c>
-      <c r="B20" s="15">
-        <v>14</v>
-      </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G20" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="13">
+        <v>16</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>15</v>
-      </c>
-      <c r="B21" s="15">
-        <v>15</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G21" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="B21" s="13">
+        <v>17</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <v>16</v>
-      </c>
-      <c r="B22" s="15">
-        <v>16</v>
-      </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" s="17">
+        <v>20</v>
+      </c>
+      <c r="B22" s="13">
+        <v>18</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <v>17</v>
-      </c>
-      <c r="B23" s="15">
-        <v>17</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="13">
+        <v>19</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
-        <v>18</v>
-      </c>
-      <c r="B24" s="15">
-        <v>18</v>
-      </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="G24" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="13">
+        <v>20</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
-        <v>19</v>
-      </c>
-      <c r="B25" s="15">
-        <v>19</v>
-      </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="G25" s="17">
+        <v>23</v>
+      </c>
+      <c r="B25" s="13">
+        <v>21</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
-        <v>20</v>
-      </c>
-      <c r="B26" s="15">
-        <v>20</v>
-      </c>
-      <c r="C26" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="13">
         <v>22</v>
       </c>
-      <c r="D26" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="C26" s="14"/>
+      <c r="D26" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
-        <v>21</v>
-      </c>
-      <c r="B27" s="15">
-        <v>21</v>
-      </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="13">
+        <v>0</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="15"/>
+      <c r="G27" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
-        <v>23</v>
-      </c>
-      <c r="B28" s="15">
-        <v>22</v>
-      </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="13">
+        <v>0</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" s="15"/>
+      <c r="G28" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>27</v>
+      </c>
+      <c r="B29" s="13">
+        <v>0</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>28</v>
+      </c>
+      <c r="B30" s="13">
+        <v>0</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E28" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="G28" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
-        <v>25</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
-        <v>26</v>
-      </c>
-      <c r="B30" s="15">
-        <v>0</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="19" t="s">
-        <v>100</v>
+      <c r="F30" s="15"/>
+      <c r="G30" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
+        <v>29</v>
+      </c>
+      <c r="B31" s="13">
+        <v>0</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="15">
-        <v>0</v>
-      </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F31" s="17"/>
-      <c r="G31" s="19" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="E31" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="15"/>
+      <c r="G31" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
-        <v>28</v>
-      </c>
-      <c r="B32" s="15">
-        <v>0</v>
-      </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F32" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="G32" s="17" t="s">
-        <v>87</v>
+        <v>30</v>
+      </c>
+      <c r="B32" s="13">
+        <v>23</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
-        <v>29</v>
-      </c>
-      <c r="B33" s="15">
-        <v>0</v>
-      </c>
-      <c r="C33" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="13">
         <v>24</v>
       </c>
-      <c r="D33" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="17" t="s">
+      <c r="C33" s="14"/>
+      <c r="D33" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
+        <v>32</v>
+      </c>
+      <c r="B34" s="13">
+        <v>25</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="4">
-        <v>30</v>
-      </c>
-      <c r="B34" s="15">
-        <v>0</v>
-      </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="F34" s="17"/>
-      <c r="G34" s="19" t="s">
-        <v>102</v>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
-        <v>31</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A36" s="4">
-        <v>32</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>62</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B35" s="13">
+        <v>26</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="4">
-        <v>33</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>63</v>
-      </c>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="C37" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
       <c r="F37" s="5"/>
-      <c r="G37" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A38" s="4">
-        <v>34</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>90</v>
-      </c>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C39" s="8" t="s">
+        <v>1</v>
+      </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="C40" s="5" t="s">
-        <v>56</v>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C40" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -1621,23 +1602,22 @@
       <c r="G40" s="5"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C41" s="8"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C42" s="10" t="s">
-        <v>1</v>
-      </c>
+      <c r="C42" s="8"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C43" s="10" t="s">
-        <v>2</v>
+      <c r="C43" s="8" t="s">
+        <v>3</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -1645,127 +1625,104 @@
       <c r="G43" s="5"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C44" s="10"/>
+      <c r="C44" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C45" s="10"/>
+      <c r="C45" s="8" t="s">
+        <v>5</v>
+      </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C46" s="10" t="s">
-        <v>3</v>
+      <c r="C46" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C47" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C48" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C49" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="E56"/>
+      <c r="F56"/>
+      <c r="G56"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="E57"/>
+      <c r="F57"/>
+      <c r="G57"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="11"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
       <c r="E58"/>
       <c r="F58"/>
       <c r="G58"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="11"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
       <c r="E59"/>
       <c r="F59"/>
       <c r="G59"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="11"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
+      <c r="A60" s="9"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
       <c r="E60"/>
       <c r="F60"/>
       <c r="G60"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="11"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
       <c r="E61"/>
       <c r="F61"/>
       <c r="G61"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="11"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
       <c r="E62"/>
       <c r="F62"/>
       <c r="G62"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="11"/>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="8"/>
       <c r="E63"/>
       <c r="F63"/>
       <c r="G63"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="11"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="E64"/>
-      <c r="F64"/>
-      <c r="G64"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="11"/>
-      <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
-      <c r="E65"/>
-      <c r="F65"/>
-      <c r="G65"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="11"/>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="10"/>
-      <c r="E66"/>
-      <c r="F66"/>
-      <c r="G66"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ya se limpio DATOS y se creó DATOS_LIMPIOS que ya están listo para ser usado en LM
</commit_message>
<xml_diff>
--- a/hipotesis/HIPOTESIS vs VARIABLES.xlsx
+++ b/hipotesis/HIPOTESIS vs VARIABLES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/MCD/proyectodegrado2/hipotesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB623382-A79F-8F43-A0A7-0C586CC45CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFB2ED3-40FE-5A4B-A58A-A8F18B01054A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19820" yWindow="1220" windowWidth="32180" windowHeight="25300" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
   </bookViews>
@@ -836,7 +836,7 @@
   <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
se estudia las correlaciones entre las variables
</commit_message>
<xml_diff>
--- a/hipotesis/HIPOTESIS vs VARIABLES.xlsx
+++ b/hipotesis/HIPOTESIS vs VARIABLES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/MCD/proyectodegrado2/hipotesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFB2ED3-40FE-5A4B-A58A-A8F18B01054A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8709B7E1-6AE2-7948-A6CC-7BE4E3836797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19820" yWindow="1220" windowWidth="32180" windowHeight="25300" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
+    <workbookView xWindow="23900" yWindow="580" windowWidth="27160" windowHeight="25300" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -431,7 +431,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,12 +441,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,23 +495,23 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -835,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39A78E9-D45D-3D4E-A52F-2B0492CA372F}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -887,39 +881,39 @@
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="13">
-        <v>0</v>
-      </c>
-      <c r="C3" s="14" t="s">
+      <c r="B3" s="14">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="13">
-        <v>0</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15" t="s">
+      <c r="B4" s="14">
+        <v>0</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="18" t="s">
         <v>88</v>
       </c>
     </row>
@@ -927,7 +921,7 @@
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="13">
         <v>1</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -948,22 +942,22 @@
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="14">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="18" t="s">
         <v>97</v>
       </c>
     </row>
@@ -971,20 +965,20 @@
       <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="14">
         <v>3</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="15" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -992,20 +986,20 @@
       <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="14">
         <v>4</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="15" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1013,20 +1007,20 @@
       <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="14">
         <v>5</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="15" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1034,20 +1028,20 @@
       <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="14">
         <v>6</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="15" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1055,18 +1049,18 @@
       <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="14">
         <v>7</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="15" t="s">
+      <c r="C11" s="14"/>
+      <c r="D11" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="17">
+      <c r="F11" s="16"/>
+      <c r="G11" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1074,18 +1068,18 @@
       <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="14">
         <v>8</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="15" t="s">
+      <c r="C12" s="14"/>
+      <c r="D12" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="17">
+      <c r="F12" s="16"/>
+      <c r="G12" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1093,18 +1087,18 @@
       <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="14">
         <v>9</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="15" t="s">
+      <c r="C13" s="14"/>
+      <c r="D13" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="17">
+      <c r="F13" s="16"/>
+      <c r="G13" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1112,20 +1106,20 @@
       <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="14">
         <v>10</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="15" t="s">
+      <c r="C14" s="14"/>
+      <c r="D14" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="G14" s="17">
+      <c r="G14" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1133,20 +1127,20 @@
       <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="14">
         <v>11</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="15" t="s">
+      <c r="C15" s="14"/>
+      <c r="D15" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="G15" s="17">
+      <c r="G15" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1154,20 +1148,20 @@
       <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="14">
         <v>12</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="15" t="s">
+      <c r="C16" s="14"/>
+      <c r="D16" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="18" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1175,20 +1169,20 @@
       <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="14">
         <v>13</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15" t="s">
+      <c r="F17" s="16"/>
+      <c r="G17" s="16" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1196,20 +1190,20 @@
       <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="14">
         <v>14</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="15" t="s">
+      <c r="C18" s="14"/>
+      <c r="D18" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1217,20 +1211,20 @@
       <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="14">
         <v>15</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="15" t="s">
+      <c r="C19" s="14"/>
+      <c r="D19" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1238,20 +1232,20 @@
       <c r="A20" s="4">
         <v>18</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="14">
         <v>16</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="15" t="s">
+      <c r="C20" s="14"/>
+      <c r="D20" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1259,20 +1253,20 @@
       <c r="A21" s="4">
         <v>19</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="14">
         <v>17</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15" t="s">
+      <c r="F21" s="16"/>
+      <c r="G21" s="16" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1280,20 +1274,20 @@
       <c r="A22" s="4">
         <v>20</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="14">
         <v>18</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="15" t="s">
+      <c r="C22" s="14"/>
+      <c r="D22" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1301,20 +1295,20 @@
       <c r="A23" s="4">
         <v>21</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="14">
         <v>19</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="15" t="s">
+      <c r="C23" s="14"/>
+      <c r="D23" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="G23" s="15">
+      <c r="G23" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1322,20 +1316,20 @@
       <c r="A24" s="4">
         <v>22</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="14">
         <v>20</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15">
+      <c r="F24" s="16"/>
+      <c r="G24" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1343,18 +1337,18 @@
       <c r="A25" s="4">
         <v>23</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="14">
         <v>21</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="15" t="s">
+      <c r="C25" s="15"/>
+      <c r="D25" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15">
+      <c r="F25" s="16"/>
+      <c r="G25" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1362,20 +1356,20 @@
       <c r="A26" s="4">
         <v>24</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="14">
         <v>22</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="15" t="s">
+      <c r="C26" s="15"/>
+      <c r="D26" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="15">
+      <c r="G26" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1383,20 +1377,20 @@
       <c r="A27" s="4">
         <v>25</v>
       </c>
-      <c r="B27" s="13">
-        <v>0</v>
-      </c>
-      <c r="C27" s="14" t="s">
+      <c r="B27" s="14">
+        <v>0</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="17" t="s">
+      <c r="F27" s="16"/>
+      <c r="G27" s="18" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1404,18 +1398,18 @@
       <c r="A28" s="4">
         <v>26</v>
       </c>
-      <c r="B28" s="13">
-        <v>0</v>
-      </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="15" t="s">
+      <c r="B28" s="14">
+        <v>0</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="F28" s="15"/>
-      <c r="G28" s="17" t="s">
+      <c r="F28" s="16"/>
+      <c r="G28" s="18" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1423,20 +1417,20 @@
       <c r="A29" s="4">
         <v>27</v>
       </c>
-      <c r="B29" s="13">
-        <v>0</v>
-      </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="15" t="s">
+      <c r="B29" s="14">
+        <v>0</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="G29" s="15" t="s">
+      <c r="G29" s="16" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1444,20 +1438,20 @@
       <c r="A30" s="4">
         <v>28</v>
       </c>
-      <c r="B30" s="13">
-        <v>0</v>
-      </c>
-      <c r="C30" s="14" t="s">
+      <c r="B30" s="14">
+        <v>0</v>
+      </c>
+      <c r="C30" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="F30" s="15"/>
-      <c r="G30" s="17" t="s">
+      <c r="F30" s="16"/>
+      <c r="G30" s="18" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1465,18 +1459,18 @@
       <c r="A31" s="4">
         <v>29</v>
       </c>
-      <c r="B31" s="13">
-        <v>0</v>
-      </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="15" t="s">
+      <c r="B31" s="14">
+        <v>0</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="F31" s="15"/>
-      <c r="G31" s="17" t="s">
+      <c r="F31" s="16"/>
+      <c r="G31" s="18" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1484,20 +1478,20 @@
       <c r="A32" s="4">
         <v>30</v>
       </c>
-      <c r="B32" s="13">
+      <c r="B32" s="14">
         <v>23</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15">
+      <c r="F32" s="16"/>
+      <c r="G32" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1505,18 +1499,18 @@
       <c r="A33" s="4">
         <v>31</v>
       </c>
-      <c r="B33" s="13">
+      <c r="B33" s="14">
         <v>24</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="15" t="s">
+      <c r="C33" s="15"/>
+      <c r="D33" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15">
+      <c r="F33" s="16"/>
+      <c r="G33" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1524,20 +1518,20 @@
       <c r="A34" s="4">
         <v>32</v>
       </c>
-      <c r="B34" s="13">
+      <c r="B34" s="14">
         <v>25</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15">
+      <c r="F34" s="16"/>
+      <c r="G34" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1545,20 +1539,20 @@
       <c r="A35" s="4">
         <v>33</v>
       </c>
-      <c r="B35" s="13">
+      <c r="B35" s="14">
         <v>26</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="15" t="s">
+      <c r="C35" s="14"/>
+      <c r="D35" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="F35" s="15" t="s">
+      <c r="F35" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G35" s="17" t="s">
+      <c r="G35" s="18" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>